<commit_message>
files added for v.2 release # v.2.1
</commit_message>
<xml_diff>
--- a/result/students.xlsx
+++ b/result/students.xlsx
@@ -7,7 +7,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test 1 2021-08-20" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test 2021-09-22" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="162913" fullCalcOnLoad="1"/>
@@ -397,10 +397,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -425,7 +425,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ABCVFATIU OIVIB 1</t>
+          <t>ABCV</t>
         </is>
       </c>
     </row>
@@ -486,6 +486,30 @@
       <c r="B8" t="inlineStr">
         <is>
           <t>BYRV</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>A001</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>ABC</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>A002</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>ACBD</t>
         </is>
       </c>
     </row>
@@ -500,7 +524,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,7 +535,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>test 1 2021-08-20</t>
+          <t>test 2021-09-22</t>
         </is>
       </c>
     </row>
@@ -530,61 +554,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>A104</t>
+          <t>C020</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>91</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>A100</t>
+          <t>A021</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>A101</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>A108</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>A111</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>A102</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>